<commit_message>
Update use cases 2nd version
Mo
</commit_message>
<xml_diff>
--- a/Design/useCases.xlsx
+++ b/Design/useCases.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhao\Documents\SCSU2014FallLenovo\531\project\design\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="9396"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>use cases</t>
   </si>
@@ -67,6 +62,12 @@
     <t>2. Check Provider Directory</t>
   </si>
   <si>
+    <t>3. Verify a service</t>
+  </si>
+  <si>
+    <t>4. Schedule service provided Report</t>
+  </si>
+  <si>
     <t>Member</t>
   </si>
   <si>
@@ -85,6 +86,12 @@
     <t>10. Update provider Directory</t>
   </si>
   <si>
+    <t>1. Generate all weekly member reports at 11:59pm Friday</t>
+  </si>
+  <si>
+    <t>2. generate all weekly provider reports at 11:59pm Friday</t>
+  </si>
+  <si>
     <t>3. Send weekly Report to member and provider</t>
   </si>
   <si>
@@ -94,37 +101,22 @@
     <t>2. Get member service report</t>
   </si>
   <si>
+    <t>5. Verify weekly service fee</t>
+  </si>
+  <si>
+    <t>6. Verify weekly recorded service</t>
+  </si>
+  <si>
+    <t>2. Schedule weekly service Report</t>
+  </si>
+  <si>
     <t>3. Process Provider Payment</t>
   </si>
   <si>
+    <t>4. Bill for Provider Services</t>
+  </si>
+  <si>
     <t>System</t>
-  </si>
-  <si>
-    <t>5. Schedule weekly service Report for member</t>
-  </si>
-  <si>
-    <t>6. Schedule service provided Report for provider</t>
-  </si>
-  <si>
-    <t>4. Verify weekly service fee</t>
-  </si>
-  <si>
-    <t>5. Verify weekly recorded service</t>
-  </si>
-  <si>
-    <t>1. Generate all weekly member reports at 11:59pm Sunday</t>
-  </si>
-  <si>
-    <t>2. generate all weekly provider reports at 11:59pm Sunday</t>
-  </si>
-  <si>
-    <t>3. Add a service record</t>
-  </si>
-  <si>
-    <t>3. Bill for Provider Services</t>
-  </si>
-  <si>
-    <t>4. Reinstate member</t>
   </si>
 </sst>
 </file>
@@ -227,7 +219,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -243,7 +235,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -285,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,7 +312,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -529,15 +521,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -564,134 +556,136 @@
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="1" t="s">
-        <v>26</v>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="B25" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="B26" s="1"/>
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B28" s="1"/>
     </row>
     <row r="29" spans="1:2">
       <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>6</v>
@@ -699,44 +693,37 @@
     </row>
     <row r="31" spans="1:2">
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>25</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="B37" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="B38" s="1"/>
+      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -754,7 +741,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>